<commit_message>
20180307We - Added relationship
</commit_message>
<xml_diff>
--- a/03_Analysis and design/Party_Organisation.xlsx
+++ b/03_Analysis and design/Party_Organisation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="1" r:id="rId1"/>
@@ -67,17 +67,6 @@
     <t>Represents a collection of people organized together into a community or other social, commercial or political structure. The group has some common purpose or reason for existence which goes beyond the set of people belonging to it and can act as an Agent. Organizations are often decomposable into hierarchical structures</t>
   </si>
   <si>
-    <t>SubClass of: foaf:Agent
-Equivalent class: foaf:Organization
-org:subOrganizationOf org:Organization
-org:transitiveSubOrganizationOf org:Organization
-org:hasSuborganizationOf org:Organization
-org:Purpose Text
-org:Classification skos:Concept
-org:Identifier skos:Notation
-org:linkedTo org:Organization</t>
-  </si>
-  <si>
     <t>UBL</t>
   </si>
   <si>
@@ -263,9 +252,6 @@
   </si>
   <si>
     <t>PROPERTIES</t>
-  </si>
-  <si>
-    <t>foaf:weblog</t>
   </si>
   <si>
     <t>MarkCareIndicator -&gt; Indicator
@@ -292,6 +278,21 @@
   </si>
   <si>
     <t>ubl:EndpointID</t>
+  </si>
+  <si>
+    <t>SubClass of: foaf:Agent
+Equivalent class: foaf:Organization
+org:subOrganizationOf org:Organization
+org:transitiveSubOrganizationOf org:Organization
+org:hasSuborganizationOf org:Organization
+org:Purpose Text
+org:Classification skos:Concept
+org:Identifier skos:Notation
+org:linkedTo org:Organization
+org:hasSite org:Site</t>
+  </si>
+  <si>
+    <t>org:hasSite (org:Site)</t>
   </si>
 </sst>
 </file>
@@ -356,27 +357,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -397,6 +377,27 @@
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -411,16 +412,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B2:H6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B2:H6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="B2:H6"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="ONTOLOGY" dataDxfId="8"/>
-    <tableColumn id="2" name="ELEMENT" dataDxfId="7"/>
-    <tableColumn id="3" name="URL DOCUMENTATION" dataDxfId="6"/>
-    <tableColumn id="4" name="DEFINITION" dataDxfId="5"/>
-    <tableColumn id="5" name="PROPERTIES" dataDxfId="4"/>
-    <tableColumn id="6" name="PROS" dataDxfId="3"/>
-    <tableColumn id="7" name="CONS" dataDxfId="2"/>
+    <tableColumn id="1" name="ONTOLOGY" dataDxfId="6"/>
+    <tableColumn id="2" name="ELEMENT" dataDxfId="5"/>
+    <tableColumn id="3" name="URL DOCUMENTATION" dataDxfId="4"/>
+    <tableColumn id="4" name="DEFINITION" dataDxfId="3"/>
+    <tableColumn id="5" name="PROPERTIES" dataDxfId="2"/>
+    <tableColumn id="6" name="PROS" dataDxfId="1"/>
+    <tableColumn id="7" name="CONS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -728,7 +729,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -744,25 +747,25 @@
   <sheetData>
     <row r="2" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="G2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -782,7 +785,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="2:8" s="1" customFormat="1" ht="210" x14ac:dyDescent="0.25">
@@ -802,13 +805,13 @@
         <v>9</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
@@ -822,32 +825,32 @@
         <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="2:8" ht="330" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -863,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E36"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,7 +881,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -887,197 +890,197 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1105,7 +1108,7 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -1113,7 +1116,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -1121,7 +1124,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -1129,7 +1132,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -1137,7 +1140,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20180307We - RegisteredOrg comparison
</commit_message>
<xml_diff>
--- a/03_Analysis and design/Party_Organisation.xlsx
+++ b/03_Analysis and design/Party_Organisation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="101">
   <si>
     <t>PPROC</t>
   </si>
@@ -293,6 +293,75 @@
   </si>
   <si>
     <t>org:hasSite (org:Site)</t>
+  </si>
+  <si>
+    <t>rov:RegisteredOrganization</t>
+  </si>
+  <si>
+    <t>ubl:PartyLegalEntity</t>
+  </si>
+  <si>
+    <t>PartyName (Name)</t>
+  </si>
+  <si>
+    <t>CompanyID (Identifier)</t>
+  </si>
+  <si>
+    <t>RegistrationDate (Date)</t>
+  </si>
+  <si>
+    <t>RegistrationExpirationDate (Date)</t>
+  </si>
+  <si>
+    <t>CompanyLegalFormCode (Code)</t>
+  </si>
+  <si>
+    <t>CompanyLegalForm (Text)</t>
+  </si>
+  <si>
+    <t>SolePropietorshipIndicator (Indicator)</t>
+  </si>
+  <si>
+    <t>CompanyLiquidationStatusCode (Code)</t>
+  </si>
+  <si>
+    <t>CorporateStockAmount (Amount)</t>
+  </si>
+  <si>
+    <t>FullyPaidSharesIndicator (Indicator)</t>
+  </si>
+  <si>
+    <t>RegistrationAddress (Address)</t>
+  </si>
+  <si>
+    <t>CorporateRegistrationScheme (CorporateRegistration)</t>
+  </si>
+  <si>
+    <t>HeadOfficeParty (Party)</t>
+  </si>
+  <si>
+    <t>ShareholderParty (ShareholderParty)</t>
+  </si>
+  <si>
+    <t>rov:LegalName</t>
+  </si>
+  <si>
+    <t>skos:altLabel</t>
+  </si>
+  <si>
+    <t>adms:Identifier</t>
+  </si>
+  <si>
+    <t>rov:registration (Identifier)</t>
+  </si>
+  <si>
+    <t>rov:orgStatus</t>
+  </si>
+  <si>
+    <t>rov:orgType</t>
+  </si>
+  <si>
+    <t>rov:orgActivity</t>
   </si>
 </sst>
 </file>
@@ -437,6 +506,17 @@
     <tableColumn id="6" name="ubl:Party"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="C39:D57" totalsRowShown="0">
+  <autoFilter ref="C39:D57"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="rov:RegisteredOrganization"/>
+    <tableColumn id="2" name="ubl:PartyLegalEntity"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -864,10 +944,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E36"/>
+  <dimension ref="B2:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,10 +1163,118 @@
         <v>75</v>
       </c>
     </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>